<commit_message>
wow haven't touched this in 2 years
</commit_message>
<xml_diff>
--- a/Books.xlsx
+++ b/Books.xlsx
@@ -1,23 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/54680535009a7d12/Folders/04 Personal/Misc-Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="25" documentId="13_ncr:1_{5E18CE11-99EE-41C1-9E53-DA422766715C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0AE23C52-AC88-4CF4-8860-9E91FB6D6B54}"/>
+  <xr:revisionPtr revIDLastSave="106" documentId="13_ncr:1_{5E18CE11-99EE-41C1-9E53-DA422766715C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{29D70B12-7599-4884-A00F-B42069A7A2FD}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="2022" sheetId="4" r:id="rId1"/>
-    <sheet name="2021" sheetId="2" r:id="rId2"/>
+    <sheet name="2024" sheetId="6" r:id="rId1"/>
+    <sheet name="2023" sheetId="5" r:id="rId2"/>
+    <sheet name="2022" sheetId="4" r:id="rId3"/>
+    <sheet name="2021" sheetId="2" r:id="rId4"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId3"/>
+    <externalReference r:id="rId5"/>
   </externalReferences>
   <definedNames>
     <definedName name="BudgetsAvailableDates">_xlfn.ANCHORARRAY(#REF!)</definedName>
@@ -51,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="64">
   <si>
     <t>Automate the Boring Stuff with Python</t>
   </si>
@@ -174,13 +176,95 @@
   </si>
   <si>
     <t>Dune 5</t>
+  </si>
+  <si>
+    <t>Chris Voss</t>
+  </si>
+  <si>
+    <t>Negotiate Like Your Life Depends on It</t>
+  </si>
+  <si>
+    <t xml:space="preserve">solid negotiation book. Would be beneficial to read again. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dune 6 </t>
+  </si>
+  <si>
+    <t>Understanding Today's Natural Gas Market</t>
+  </si>
+  <si>
+    <t>Bob Shively</t>
+  </si>
+  <si>
+    <t>Understanding Today's Electricity Markets</t>
+  </si>
+  <si>
+    <t>Show Your Work</t>
+  </si>
+  <si>
+    <t>Austin Kleon</t>
+  </si>
+  <si>
+    <t>The Grid</t>
+  </si>
+  <si>
+    <t>Gretchen Bakke P.h.d</t>
+  </si>
+  <si>
+    <t>Harry Potter and the Methods of Rationality</t>
+  </si>
+  <si>
+    <t>Eliezer Yudkowsky</t>
+  </si>
+  <si>
+    <t>*****</t>
+  </si>
+  <si>
+    <t xml:space="preserve">never read a fan fic before. I loved this book. Reminded me how cool harry potter is. Eliezer is a talented writer. </t>
+  </si>
+  <si>
+    <t>the Prophet</t>
+  </si>
+  <si>
+    <t>Kahlil Gibran</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">a 'soul alignment' type book. Similar feeling after reading to </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>The Alchemist</t>
+    </r>
+  </si>
+  <si>
+    <t>The 3 body Problem</t>
+  </si>
+  <si>
+    <t>Cixin Liu</t>
+  </si>
+  <si>
+    <t>I enjoyed this book. Best sci-fi I've read since Dune. I like when futurism has truth and philosophy. Strategic too</t>
+  </si>
+  <si>
+    <t>The Dark Forest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">great ending to the problem that seemed so impossible. While hiding the strategy from the reader until the end, just like the aliens, I was fooled. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -190,6 +274,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -217,7 +309,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -227,6 +319,14 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -236,7 +336,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -244,6 +343,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -282,7 +382,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Snapshot"/>
@@ -1489,9 +1589,13 @@
 </externalLink>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{452D6498-F27B-43C8-864A-531F6A53D002}" name="Table2" displayName="Table2" ref="A1:F10" totalsRowShown="0">
-  <autoFilter ref="A1:F10" xr:uid="{60EEE120-0293-4558-986C-F748A4731A50}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{452D6498-F27B-43C8-864A-531F6A53D002}" name="Table2" displayName="Table2" ref="A1:F17" totalsRowShown="0">
+  <autoFilter ref="A1:F17" xr:uid="{60EEE120-0293-4558-986C-F748A4731A50}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{B1255BCD-213F-4CE4-91E0-A514A76AE913}" name="Title:"/>
     <tableColumn id="2" xr3:uid="{A668F299-58FB-4739-9138-873384DC7022}" name="Author:"/>
@@ -1505,15 +1609,15 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{40CD5C28-7AEE-423B-AC6B-4D71CB04EECC}" name="Table5" displayName="Table5" ref="A1:F6" totalsRowShown="0" dataDxfId="0" headerRowBorderDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{40CD5C28-7AEE-423B-AC6B-4D71CB04EECC}" name="Table5" displayName="Table5" ref="A1:F6" totalsRowShown="0" dataDxfId="6" headerRowBorderDxfId="7">
   <autoFilter ref="A1:F6" xr:uid="{45D8D199-C79F-42B0-BA79-59BD62B9F4C1}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{C222D202-2E88-4127-B100-F48441F6A61E}" name="Title:" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{B98A22D6-88AA-4BDF-BF44-A3782AAAB96F}" name="Author:" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{CC6DDD3E-54FA-446E-8330-2CFDD361C614}" name="Date Started: " dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{4318F825-486D-4EB2-9062-BFC5B2A3EFC7}" name="Date Finished:" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{1918FEBD-AA67-44C5-9A96-7F4499969656}" name="Rating:" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{46096A80-E7C7-4E20-A57F-2091310078B3}" name="Notes:" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{C222D202-2E88-4127-B100-F48441F6A61E}" name="Title:" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{B98A22D6-88AA-4BDF-BF44-A3782AAAB96F}" name="Author:" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{CC6DDD3E-54FA-446E-8330-2CFDD361C614}" name="Date Started: " dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{4318F825-486D-4EB2-9062-BFC5B2A3EFC7}" name="Date Finished:" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{1918FEBD-AA67-44C5-9A96-7F4499969656}" name="Rating:" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{46096A80-E7C7-4E20-A57F-2091310078B3}" name="Notes:" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1781,24 +1885,201 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D77D881-EC9E-4F0B-9BE8-27C360AC1061}">
-  <dimension ref="A1:F10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E29B7019-4D0F-4782-A19D-2B10FF4895A8}">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="40.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="133.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" s="9">
+        <v>45296</v>
+      </c>
+      <c r="D2" s="9">
+        <v>45323</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" s="3">
+        <v>45323</v>
+      </c>
+      <c r="D3" s="3">
+        <v>45337</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E1048576" xr:uid="{D2D7B34B-7526-4309-9596-AF446D76884D}">
+      <formula1>"*,**,***,****,*****"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4F2AB4F-4E5B-4A2B-9FBF-0CDE67AB80FC}">
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="46.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.109375" customWidth="1"/>
-    <col min="4" max="4" width="15.88671875" customWidth="1"/>
-    <col min="5" max="5" width="9.33203125" customWidth="1"/>
-    <col min="6" max="6" width="103.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="102.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" s="9">
+        <v>44927</v>
+      </c>
+      <c r="D2" s="9">
+        <v>44958</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3" s="12">
+        <v>44958</v>
+      </c>
+      <c r="D3" s="12">
+        <v>45352</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E1048576" xr:uid="{777FF739-39FD-4FB8-94C2-EB6013CF9673}">
+      <formula1>"*,**,***,****,*****"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D77D881-EC9E-4F0B-9BE8-27C360AC1061}">
+  <dimension ref="A1:F16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="46.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" customWidth="1"/>
+    <col min="5" max="5" width="9.28515625" customWidth="1"/>
+    <col min="6" max="6" width="103.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>30</v>
       </c>
@@ -1818,7 +2099,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1835,7 +2116,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1852,7 +2133,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -1869,7 +2150,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -1886,7 +2167,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>33</v>
       </c>
@@ -1903,7 +2184,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -1920,7 +2201,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -1940,7 +2221,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>39</v>
       </c>
@@ -1957,7 +2238,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>40</v>
       </c>
@@ -1974,9 +2255,114 @@
         <v>8</v>
       </c>
     </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" s="3">
+        <v>44787</v>
+      </c>
+      <c r="D11" s="3">
+        <v>44795</v>
+      </c>
+      <c r="E11" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="3">
+        <v>44803</v>
+      </c>
+      <c r="D12" s="3">
+        <v>44859</v>
+      </c>
+      <c r="E12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" s="3">
+        <v>44803</v>
+      </c>
+      <c r="D13" s="3">
+        <v>44859</v>
+      </c>
+      <c r="E13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14" s="3">
+        <v>44803</v>
+      </c>
+      <c r="D14" s="3">
+        <v>44859</v>
+      </c>
+      <c r="E14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15" t="s">
+        <v>49</v>
+      </c>
+      <c r="C15" s="3">
+        <v>44860</v>
+      </c>
+      <c r="D15" s="3">
+        <v>44864</v>
+      </c>
+      <c r="E15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>50</v>
+      </c>
+      <c r="B16" t="s">
+        <v>51</v>
+      </c>
+      <c r="C16" s="3">
+        <v>44866</v>
+      </c>
+      <c r="D16" s="3">
+        <v>44922</v>
+      </c>
+      <c r="E16" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E10" xr:uid="{46FDD7B0-E21C-41D8-8E36-E8DB6FC4625D}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E16" xr:uid="{46FDD7B0-E21C-41D8-8E36-E8DB6FC4625D}">
       <formula1>"*,**,***,****,*****"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1987,29 +2373,27 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA2570D6-559C-4534-AA5B-101E6CBF68B0}">
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:F8"/>
-    </sheetView>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="46.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="13.88671875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="46.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" style="1" customWidth="1"/>
     <col min="5" max="5" width="12" style="1" customWidth="1"/>
-    <col min="6" max="6" width="103.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.109375" style="1"/>
-    <col min="8" max="8" width="37.109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="21.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.109375" style="1"/>
+    <col min="6" max="6" width="103.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="1"/>
+    <col min="8" max="8" width="37.140625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="21.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>30</v>
       </c>
@@ -2031,7 +2415,7 @@
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>24</v>
       </c>
@@ -2051,7 +2435,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -2071,7 +2455,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -2091,7 +2475,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -2111,7 +2495,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
added Death's End by Cixin Liu
</commit_message>
<xml_diff>
--- a/Books.xlsx
+++ b/Books.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/54680535009a7d12/Folders/04 Personal/Misc-Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kparsons\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="106" documentId="13_ncr:1_{5E18CE11-99EE-41C1-9E53-DA422766715C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{29D70B12-7599-4884-A00F-B42069A7A2FD}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{60A710AE-15FA-415B-9115-6E65E26A451D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-255" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2024" sheetId="6" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="66">
   <si>
     <t>Automate the Boring Stuff with Python</t>
   </si>
@@ -258,6 +258,12 @@
   </si>
   <si>
     <t xml:space="preserve">great ending to the problem that seemed so impossible. While hiding the strategy from the reader until the end, just like the aliens, I was fooled. </t>
+  </si>
+  <si>
+    <t>Death's End</t>
+  </si>
+  <si>
+    <t>each book had a wild ending. Great series. Made me more scared of the universe whilst wishing lightspeed travel become a reality for humanity</t>
   </si>
 </sst>
 </file>
@@ -309,7 +315,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -319,14 +325,7 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1587,10 +1586,6 @@
     </sheetDataSet>
   </externalBook>
 </externalLink>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1886,10 +1881,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E29B7019-4D0F-4782-A19D-2B10FF4895A8}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1898,47 +1893,47 @@
     <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="133.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="4" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" t="s">
         <v>59</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" t="s">
         <v>60</v>
       </c>
-      <c r="C2" s="9">
+      <c r="C2" s="3">
         <v>45296</v>
       </c>
-      <c r="D2" s="9">
+      <c r="D2" s="3">
         <v>45323</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1946,7 +1941,7 @@
       <c r="A3" t="s">
         <v>62</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" t="s">
         <v>60</v>
       </c>
       <c r="C3" s="3">
@@ -1955,11 +1950,31 @@
       <c r="D3" s="3">
         <v>45337</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" t="s">
         <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C4" s="3">
+        <v>45338</v>
+      </c>
+      <c r="D4" s="3">
+        <v>45365</v>
+      </c>
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1976,8 +1991,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4F2AB4F-4E5B-4A2B-9FBF-0CDE67AB80FC}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1986,67 +2001,67 @@
     <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="102.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="4" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" t="s">
         <v>52</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" t="s">
         <v>53</v>
       </c>
-      <c r="C2" s="9">
+      <c r="C2" s="3">
         <v>44927</v>
       </c>
-      <c r="D2" s="9">
+      <c r="D2" s="3">
         <v>44958</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" t="s">
         <v>54</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
+      <c r="A3" t="s">
         <v>56</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" t="s">
         <v>57</v>
       </c>
-      <c r="C3" s="12">
+      <c r="C3" s="3">
         <v>44958</v>
       </c>
-      <c r="D3" s="12">
+      <c r="D3" s="3">
         <v>45352</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" t="s">
         <v>58</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added Murderbot diaries book 1
</commit_message>
<xml_diff>
--- a/Books.xlsx
+++ b/Books.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kparsons\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{60A710AE-15FA-415B-9115-6E65E26A451D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F553A70D-98DB-42A8-B07F-AC4B51AD2950}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-255" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1275" yWindow="-120" windowWidth="27645" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2024" sheetId="6" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="69">
   <si>
     <t>Automate the Boring Stuff with Python</t>
   </si>
@@ -264,6 +264,15 @@
   </si>
   <si>
     <t>each book had a wild ending. Great series. Made me more scared of the universe whilst wishing lightspeed travel become a reality for humanity</t>
+  </si>
+  <si>
+    <t>All Systems Red (murderbot diaries)</t>
+  </si>
+  <si>
+    <t>Martha Wells</t>
+  </si>
+  <si>
+    <t xml:space="preserve">First person story about a combination of machine and human biology might "feel" like. What ratio of biology to machine (assuming machine is unconsious) is it slavey? </t>
   </si>
 </sst>
 </file>
@@ -303,7 +312,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -311,11 +320,122 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -326,11 +446,217 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="20">
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1589,13 +1915,28 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{3C15E0FB-2493-4B06-8F83-E22386A3E6CF}" name="Table3" displayName="Table3" ref="A1:F5" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="7" tableBorderDxfId="8" totalsRowBorderDxfId="6">
+  <autoFilter ref="A1:F5" xr:uid="{3C15E0FB-2493-4B06-8F83-E22386A3E6CF}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{E8265B0B-A584-4581-9585-6612A023A6BE}" name="Title:" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{4E7572E3-9EF1-43F5-A490-6781D368479E}" name="Author:" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{8573FB8A-8D48-492D-AF36-575F8CA4B6C5}" name="Date Started: " dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{2AC2B52F-ECDA-4759-9914-680384661173}" name="Date Finished:" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{FD550F85-677B-468B-8E07-194FA0DD48DA}" name="Rating:" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{BC9F5372-8694-430F-9309-2C57EE0444FC}" name="Notes:" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{452D6498-F27B-43C8-864A-531F6A53D002}" name="Table2" displayName="Table2" ref="A1:F17" totalsRowShown="0">
   <autoFilter ref="A1:F17" xr:uid="{60EEE120-0293-4558-986C-F748A4731A50}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{B1255BCD-213F-4CE4-91E0-A514A76AE913}" name="Title:"/>
     <tableColumn id="2" xr3:uid="{A668F299-58FB-4739-9138-873384DC7022}" name="Author:"/>
-    <tableColumn id="3" xr3:uid="{E5572243-B8EF-4FCD-9A5A-BE1494245E11}" name="Date Started: " dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{D84211BE-699A-4173-BC97-15CB00259096}" name="Date Finished:" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{E5572243-B8EF-4FCD-9A5A-BE1494245E11}" name="Date Started: " dataDxfId="19"/>
+    <tableColumn id="4" xr3:uid="{D84211BE-699A-4173-BC97-15CB00259096}" name="Date Finished:" dataDxfId="18"/>
     <tableColumn id="5" xr3:uid="{7E5034D1-A953-4DDF-BC62-F13A781B9087}" name="Rating:"/>
     <tableColumn id="6" xr3:uid="{68BAB37A-D0B2-427D-B2C2-08686F332AAB}" name="Notes:"/>
   </tableColumns>
@@ -1603,16 +1944,16 @@
 </table>
 </file>
 
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{40CD5C28-7AEE-423B-AC6B-4D71CB04EECC}" name="Table5" displayName="Table5" ref="A1:F6" totalsRowShown="0" dataDxfId="6" headerRowBorderDxfId="7">
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{40CD5C28-7AEE-423B-AC6B-4D71CB04EECC}" name="Table5" displayName="Table5" ref="A1:F6" totalsRowShown="0" dataDxfId="16" headerRowBorderDxfId="17">
   <autoFilter ref="A1:F6" xr:uid="{45D8D199-C79F-42B0-BA79-59BD62B9F4C1}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{C222D202-2E88-4127-B100-F48441F6A61E}" name="Title:" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{B98A22D6-88AA-4BDF-BF44-A3782AAAB96F}" name="Author:" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{CC6DDD3E-54FA-446E-8330-2CFDD361C614}" name="Date Started: " dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{4318F825-486D-4EB2-9062-BFC5B2A3EFC7}" name="Date Finished:" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{1918FEBD-AA67-44C5-9A96-7F4499969656}" name="Rating:" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{46096A80-E7C7-4E20-A57F-2091310078B3}" name="Notes:" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{C222D202-2E88-4127-B100-F48441F6A61E}" name="Title:" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{B98A22D6-88AA-4BDF-BF44-A3782AAAB96F}" name="Author:" dataDxfId="14"/>
+    <tableColumn id="6" xr3:uid="{CC6DDD3E-54FA-446E-8330-2CFDD361C614}" name="Date Started: " dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{4318F825-486D-4EB2-9062-BFC5B2A3EFC7}" name="Date Finished:" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{1918FEBD-AA67-44C5-9A96-7F4499969656}" name="Rating:" dataDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{46096A80-E7C7-4E20-A57F-2091310078B3}" name="Notes:" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1881,100 +2222,120 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E29B7019-4D0F-4782-A19D-2B10FF4895A8}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="40.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="133.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" customWidth="1"/>
+    <col min="5" max="5" width="9.28515625" customWidth="1"/>
+    <col min="6" max="6" width="153.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="11" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="7">
         <v>45296</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="7">
         <v>45323</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="13" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="7">
         <v>45323</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="7">
         <v>45337</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="13" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="16">
         <v>45338</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="16">
         <v>45365</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="17" t="s">
         <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="C5" s="16">
+        <v>45438</v>
+      </c>
+      <c r="D5" s="16">
+        <v>45440</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="17" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1984,6 +2345,9 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -1991,9 +2355,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4F2AB4F-4E5B-4A2B-9FBF-0CDE67AB80FC}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2081,7 +2443,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="A2" sqref="A2:F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2115,265 +2477,278 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="7">
         <v>44530</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="7">
         <v>44581</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="6" t="s">
         <v>8</v>
       </c>
+      <c r="F2" s="6"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="7">
         <v>44515</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="7">
         <v>44617</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="6" t="s">
         <v>16</v>
       </c>
+      <c r="F3" s="6"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="7">
         <v>44602</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="7">
         <v>44606</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="6" t="s">
         <v>8</v>
       </c>
+      <c r="F4" s="6"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="7">
         <v>44608</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="7">
         <v>44640</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="6" t="s">
         <v>8</v>
       </c>
+      <c r="F5" s="6"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="7">
         <v>44617</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="7">
         <v>44640</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="6" t="s">
         <v>12</v>
       </c>
+      <c r="F6" s="6"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="7">
         <v>44641</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="7">
         <v>44673</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="6" t="s">
         <v>8</v>
       </c>
+      <c r="F7" s="6"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="7">
         <v>44641</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="7">
         <v>44687</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="6" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="7">
         <v>44688</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="7">
         <v>44706</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="6" t="s">
         <v>8</v>
       </c>
+      <c r="F9" s="6"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="7">
         <v>44706</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="7">
         <v>44712</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="6" t="s">
         <v>8</v>
       </c>
+      <c r="F10" s="6"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="7">
         <v>44787</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11" s="7">
         <v>44795</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="6" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="7">
         <v>44803</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12" s="7">
         <v>44859</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="6" t="s">
         <v>8</v>
       </c>
+      <c r="F12" s="6"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13" s="7">
         <v>44803</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D13" s="7">
         <v>44859</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="6" t="s">
         <v>8</v>
       </c>
+      <c r="F13" s="6"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="A14" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="7">
         <v>44803</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14" s="7">
         <v>44859</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="6" t="s">
         <v>8</v>
       </c>
+      <c r="F14" s="6"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="A15" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C15" s="7">
         <v>44860</v>
       </c>
-      <c r="D15" s="3">
+      <c r="D15" s="7">
         <v>44864</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="6" t="s">
         <v>12</v>
       </c>
+      <c r="F15" s="6"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="A16" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="C16" s="3">
+      <c r="C16" s="7">
         <v>44866</v>
       </c>
-      <c r="D16" s="3">
+      <c r="D16" s="7">
         <v>44922</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="6" t="s">
         <v>8</v>
       </c>
+      <c r="F16" s="6"/>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -2392,7 +2767,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA2570D6-559C-4534-AA5B-101E6CBF68B0}">
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
added man's search for meaning
</commit_message>
<xml_diff>
--- a/Books.xlsx
+++ b/Books.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10311"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kparsons\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kodyparsons/Desktop/Misc-Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F553A70D-98DB-42A8-B07F-AC4B51AD2950}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CE7E880-E762-0245-9312-09839DAB06FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1275" yWindow="-120" windowWidth="27645" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1280" yWindow="680" windowWidth="27640" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2024" sheetId="6" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="72">
   <si>
     <t>Automate the Boring Stuff with Python</t>
   </si>
@@ -273,6 +273,15 @@
   </si>
   <si>
     <t xml:space="preserve">First person story about a combination of machine and human biology might "feel" like. What ratio of biology to machine (assuming machine is unconsious) is it slavey? </t>
+  </si>
+  <si>
+    <t>Man's Search for Meaning</t>
+  </si>
+  <si>
+    <t>Victor Frankl</t>
+  </si>
+  <si>
+    <t>good book overall</t>
   </si>
 </sst>
 </file>
@@ -464,6 +473,42 @@
   </cellStyles>
   <dxfs count="20">
     <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
+    </dxf>
+    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -506,7 +551,7 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -529,7 +574,7 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -601,23 +646,23 @@
       </border>
     </dxf>
     <dxf>
-      <border>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
+      <border>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -656,42 +701,6 @@
           <color indexed="64"/>
         </horizontal>
       </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1915,15 +1924,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{3C15E0FB-2493-4B06-8F83-E22386A3E6CF}" name="Table3" displayName="Table3" ref="A1:F5" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="7" tableBorderDxfId="8" totalsRowBorderDxfId="6">
-  <autoFilter ref="A1:F5" xr:uid="{3C15E0FB-2493-4B06-8F83-E22386A3E6CF}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{3C15E0FB-2493-4B06-8F83-E22386A3E6CF}" name="Table3" displayName="Table3" ref="A1:F6" totalsRowShown="0" headerRowDxfId="19" headerRowBorderDxfId="18" tableBorderDxfId="17" totalsRowBorderDxfId="16">
+  <autoFilter ref="A1:F6" xr:uid="{3C15E0FB-2493-4B06-8F83-E22386A3E6CF}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{E8265B0B-A584-4581-9585-6612A023A6BE}" name="Title:" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{4E7572E3-9EF1-43F5-A490-6781D368479E}" name="Author:" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{8573FB8A-8D48-492D-AF36-575F8CA4B6C5}" name="Date Started: " dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{2AC2B52F-ECDA-4759-9914-680384661173}" name="Date Finished:" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{FD550F85-677B-468B-8E07-194FA0DD48DA}" name="Rating:" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{BC9F5372-8694-430F-9309-2C57EE0444FC}" name="Notes:" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{E8265B0B-A584-4581-9585-6612A023A6BE}" name="Title:" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{4E7572E3-9EF1-43F5-A490-6781D368479E}" name="Author:" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{8573FB8A-8D48-492D-AF36-575F8CA4B6C5}" name="Date Started: " dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{2AC2B52F-ECDA-4759-9914-680384661173}" name="Date Finished:" dataDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{FD550F85-677B-468B-8E07-194FA0DD48DA}" name="Rating:" dataDxfId="11"/>
+    <tableColumn id="6" xr3:uid="{BC9F5372-8694-430F-9309-2C57EE0444FC}" name="Notes:" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1935,8 +1944,8 @@
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{B1255BCD-213F-4CE4-91E0-A514A76AE913}" name="Title:"/>
     <tableColumn id="2" xr3:uid="{A668F299-58FB-4739-9138-873384DC7022}" name="Author:"/>
-    <tableColumn id="3" xr3:uid="{E5572243-B8EF-4FCD-9A5A-BE1494245E11}" name="Date Started: " dataDxfId="19"/>
-    <tableColumn id="4" xr3:uid="{D84211BE-699A-4173-BC97-15CB00259096}" name="Date Finished:" dataDxfId="18"/>
+    <tableColumn id="3" xr3:uid="{E5572243-B8EF-4FCD-9A5A-BE1494245E11}" name="Date Started: " dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{D84211BE-699A-4173-BC97-15CB00259096}" name="Date Finished:" dataDxfId="8"/>
     <tableColumn id="5" xr3:uid="{7E5034D1-A953-4DDF-BC62-F13A781B9087}" name="Rating:"/>
     <tableColumn id="6" xr3:uid="{68BAB37A-D0B2-427D-B2C2-08686F332AAB}" name="Notes:"/>
   </tableColumns>
@@ -1945,15 +1954,15 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{40CD5C28-7AEE-423B-AC6B-4D71CB04EECC}" name="Table5" displayName="Table5" ref="A1:F6" totalsRowShown="0" dataDxfId="16" headerRowBorderDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{40CD5C28-7AEE-423B-AC6B-4D71CB04EECC}" name="Table5" displayName="Table5" ref="A1:F6" totalsRowShown="0" dataDxfId="6" headerRowBorderDxfId="7">
   <autoFilter ref="A1:F6" xr:uid="{45D8D199-C79F-42B0-BA79-59BD62B9F4C1}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{C222D202-2E88-4127-B100-F48441F6A61E}" name="Title:" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{B98A22D6-88AA-4BDF-BF44-A3782AAAB96F}" name="Author:" dataDxfId="14"/>
-    <tableColumn id="6" xr3:uid="{CC6DDD3E-54FA-446E-8330-2CFDD361C614}" name="Date Started: " dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{4318F825-486D-4EB2-9062-BFC5B2A3EFC7}" name="Date Finished:" dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{1918FEBD-AA67-44C5-9A96-7F4499969656}" name="Rating:" dataDxfId="11"/>
-    <tableColumn id="5" xr3:uid="{46096A80-E7C7-4E20-A57F-2091310078B3}" name="Notes:" dataDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{C222D202-2E88-4127-B100-F48441F6A61E}" name="Title:" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{B98A22D6-88AA-4BDF-BF44-A3782AAAB96F}" name="Author:" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{CC6DDD3E-54FA-446E-8330-2CFDD361C614}" name="Date Started: " dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{4318F825-486D-4EB2-9062-BFC5B2A3EFC7}" name="Date Finished:" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{1918FEBD-AA67-44C5-9A96-7F4499969656}" name="Rating:" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{46096A80-E7C7-4E20-A57F-2091310078B3}" name="Notes:" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2222,23 +2231,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E29B7019-4D0F-4782-A19D-2B10FF4895A8}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="40.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" customWidth="1"/>
-    <col min="5" max="5" width="9.28515625" customWidth="1"/>
-    <col min="6" max="6" width="153.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.1640625" customWidth="1"/>
+    <col min="4" max="4" width="15.83203125" customWidth="1"/>
+    <col min="5" max="5" width="9.33203125" customWidth="1"/>
+    <col min="6" max="6" width="153.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>30</v>
       </c>
@@ -2258,7 +2267,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
         <v>59</v>
       </c>
@@ -2278,7 +2287,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
         <v>62</v>
       </c>
@@ -2298,7 +2307,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
         <v>64</v>
       </c>
@@ -2318,7 +2327,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>66</v>
       </c>
@@ -2336,6 +2345,26 @@
       </c>
       <c r="F5" s="17" t="s">
         <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="C6" s="16">
+        <v>45474</v>
+      </c>
+      <c r="D6" s="16">
+        <v>45519</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="17" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -2357,17 +2386,17 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="40.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="102.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="102.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>30</v>
       </c>
@@ -2387,7 +2416,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>52</v>
       </c>
@@ -2407,7 +2436,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>56</v>
       </c>
@@ -2446,17 +2475,17 @@
       <selection activeCell="A2" sqref="A2:F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="46.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" customWidth="1"/>
-    <col min="5" max="5" width="9.28515625" customWidth="1"/>
-    <col min="6" max="6" width="103.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="46.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.1640625" customWidth="1"/>
+    <col min="4" max="4" width="15.83203125" customWidth="1"/>
+    <col min="5" max="5" width="9.33203125" customWidth="1"/>
+    <col min="6" max="6" width="103.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>30</v>
       </c>
@@ -2476,7 +2505,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>6</v>
       </c>
@@ -2494,7 +2523,7 @@
       </c>
       <c r="F2" s="6"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
@@ -2512,7 +2541,7 @@
       </c>
       <c r="F3" s="6"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>31</v>
       </c>
@@ -2530,7 +2559,7 @@
       </c>
       <c r="F4" s="6"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>0</v>
       </c>
@@ -2548,7 +2577,7 @@
       </c>
       <c r="F5" s="6"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>33</v>
       </c>
@@ -2566,7 +2595,7 @@
       </c>
       <c r="F6" s="6"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>35</v>
       </c>
@@ -2584,7 +2613,7 @@
       </c>
       <c r="F7" s="6"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>2</v>
       </c>
@@ -2604,7 +2633,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>39</v>
       </c>
@@ -2622,7 +2651,7 @@
       </c>
       <c r="F9" s="6"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
         <v>40</v>
       </c>
@@ -2640,7 +2669,7 @@
       </c>
       <c r="F10" s="6"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
         <v>42</v>
       </c>
@@ -2660,7 +2689,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
         <v>44</v>
       </c>
@@ -2678,7 +2707,7 @@
       </c>
       <c r="F12" s="6"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
         <v>45</v>
       </c>
@@ -2696,7 +2725,7 @@
       </c>
       <c r="F13" s="6"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
         <v>47</v>
       </c>
@@ -2714,7 +2743,7 @@
       </c>
       <c r="F14" s="6"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
         <v>48</v>
       </c>
@@ -2732,7 +2761,7 @@
       </c>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
         <v>50</v>
       </c>
@@ -2771,21 +2800,21 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="46.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="46.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="13.83203125" style="1" customWidth="1"/>
     <col min="5" max="5" width="12" style="1" customWidth="1"/>
-    <col min="6" max="6" width="103.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" style="1"/>
-    <col min="8" max="8" width="37.140625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="21.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="1"/>
+    <col min="6" max="6" width="103.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.1640625" style="1"/>
+    <col min="8" max="8" width="37.1640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="21.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>30</v>
       </c>
@@ -2807,7 +2836,7 @@
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>24</v>
       </c>
@@ -2827,7 +2856,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -2847,7 +2876,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -2867,7 +2896,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -2887,7 +2916,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
added stats and energy book
</commit_message>
<xml_diff>
--- a/Books.xlsx
+++ b/Books.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kodyparsons/Desktop/Misc-Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CE7E880-E762-0245-9312-09839DAB06FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{163936D6-3192-3D49-A5F9-4B64C581C100}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1280" yWindow="680" windowWidth="27640" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="79">
   <si>
     <t>Automate the Boring Stuff with Python</t>
   </si>
@@ -283,11 +283,35 @@
   <si>
     <t>good book overall</t>
   </si>
+  <si>
+    <t>David SpiegelHalter</t>
+  </si>
+  <si>
+    <t>The Art of Statistics</t>
+  </si>
+  <si>
+    <t>for a statistics book, it was pretty good. But still tough to get through frankly</t>
+  </si>
+  <si>
+    <t>Energy Trading &amp; Risk Management</t>
+  </si>
+  <si>
+    <t>Steven Berley</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">this book was overly vague the whole time. I can't say I got a lot from it. </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -444,7 +468,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -467,6 +491,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1924,8 +1949,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{3C15E0FB-2493-4B06-8F83-E22386A3E6CF}" name="Table3" displayName="Table3" ref="A1:F6" totalsRowShown="0" headerRowDxfId="19" headerRowBorderDxfId="18" tableBorderDxfId="17" totalsRowBorderDxfId="16">
-  <autoFilter ref="A1:F6" xr:uid="{3C15E0FB-2493-4B06-8F83-E22386A3E6CF}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{3C15E0FB-2493-4B06-8F83-E22386A3E6CF}" name="Table3" displayName="Table3" ref="A1:F8" totalsRowShown="0" headerRowDxfId="19" headerRowBorderDxfId="18" tableBorderDxfId="17" totalsRowBorderDxfId="16">
+  <autoFilter ref="A1:F8" xr:uid="{3C15E0FB-2493-4B06-8F83-E22386A3E6CF}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{E8265B0B-A584-4581-9585-6612A023A6BE}" name="Title:" dataDxfId="15"/>
     <tableColumn id="2" xr3:uid="{4E7572E3-9EF1-43F5-A490-6781D368479E}" name="Author:" dataDxfId="14"/>
@@ -2231,10 +2256,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E29B7019-4D0F-4782-A19D-2B10FF4895A8}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2365,6 +2390,46 @@
       </c>
       <c r="F6" s="17" t="s">
         <v>71</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="C7" s="18">
+        <v>45522</v>
+      </c>
+      <c r="D7" s="18">
+        <v>45609</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="17" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="C8" s="18">
+        <v>45547</v>
+      </c>
+      <c r="D8" s="18">
+        <v>45607</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="F8" s="17" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
read first book of 2025
</commit_message>
<xml_diff>
--- a/Books.xlsx
+++ b/Books.xlsx
@@ -1,25 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10720"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kodyparsons/Desktop/Misc-Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E581D324-073F-C644-BA23-21509332EDAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A31ECC3E-DCA7-C943-B7D9-DB69DC72C13B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1280" yWindow="680" windowWidth="27640" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="2024" sheetId="6" r:id="rId1"/>
-    <sheet name="2023" sheetId="5" r:id="rId2"/>
-    <sheet name="2022" sheetId="4" r:id="rId3"/>
-    <sheet name="2021" sheetId="2" r:id="rId4"/>
+    <sheet name="2025" sheetId="7" r:id="rId1"/>
+    <sheet name="2024" sheetId="6" r:id="rId2"/>
+    <sheet name="2023" sheetId="5" r:id="rId3"/>
+    <sheet name="2022" sheetId="4" r:id="rId4"/>
+    <sheet name="2021" sheetId="2" r:id="rId5"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId5"/>
+    <externalReference r:id="rId6"/>
   </externalReferences>
   <definedNames>
     <definedName name="BudgetsAvailableDates">_xlfn.ANCHORARRAY(#REF!)</definedName>
@@ -53,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="85">
   <si>
     <t>Automate the Boring Stuff with Python</t>
   </si>
@@ -312,6 +313,15 @@
   </si>
   <si>
     <t xml:space="preserve">great book. Made me think. First book to hook me in a while. </t>
+  </si>
+  <si>
+    <t>Project Hail Mary</t>
+  </si>
+  <si>
+    <t>Andy Weir</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unfortunately my first book of the year. Wayyy behind. I've started like 8 books this year that I've gotten 50 pages into and set down. This book was great! First book I "devoured" in quite a while. It's a great feeling to be hooked in a book. </t>
   </si>
 </sst>
 </file>
@@ -346,12 +356,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor theme="0" tint="-0.14999847407452621"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="10">
@@ -477,7 +493,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -501,6 +517,10 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2264,11 +2284,79 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{817434E7-1A56-8F48-BEE9-CB400449463A}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="24.1640625" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" customWidth="1"/>
+    <col min="3" max="3" width="17.83203125" customWidth="1"/>
+    <col min="4" max="4" width="12.5" customWidth="1"/>
+    <col min="5" max="5" width="9.83203125" customWidth="1"/>
+    <col min="6" max="6" width="85.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="C2" s="22">
+        <v>45846</v>
+      </c>
+      <c r="D2" s="22">
+        <v>45851</v>
+      </c>
+      <c r="E2" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="21" t="s">
+        <v>84</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2" xr:uid="{52305876-EF83-A644-968E-DA5D8EA503A2}">
+      <formula1>"*,**,***,****,*****"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E29B7019-4D0F-4782-A19D-2B10FF4895A8}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection sqref="A1:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2468,13 +2556,14 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4F2AB4F-4E5B-4A2B-9FBF-0CDE67AB80FC}">
   <dimension ref="A1:F3"/>
   <sheetViews>
@@ -2561,7 +2650,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D77D881-EC9E-4F0B-9BE8-27C360AC1061}">
   <dimension ref="A1:F16"/>
   <sheetViews>
@@ -2886,7 +2975,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA2570D6-559C-4534-AA5B-101E6CBF68B0}">
   <dimension ref="A1:I6"/>
   <sheetViews>

</xml_diff>